<commit_message>
hierarchy upload delete record changes
</commit_message>
<xml_diff>
--- a/Source/SSCore/src/test/resources/testCSV.xlsx
+++ b/Source/SSCore/src/test/resources/testCSV.xlsx
@@ -2693,7 +2693,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4693,8 +4693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6687,7 +6687,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>